<commit_message>
Oleg babak - New Smoke tests user added
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C777221
</commit_message>
<xml_diff>
--- a/PPIUK-SmokeTest/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-SmokeTest/src/test/resources/CobaltUsers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="288">
   <si>
     <t>UserName</t>
   </si>
@@ -874,6 +874,12 @@
   </si>
   <si>
     <t>GlobalPagesUser6@mailinator.com</t>
+  </si>
+  <si>
+    <t>Oleg_Babak</t>
+  </si>
+  <si>
+    <t>Password1!</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1056,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1085,7 +1091,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1294,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G119"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,10 +1912,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>75</v>
+        <v>286</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>52</v>
+        <v>287</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
@@ -1925,26 +1931,26 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E32" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>82</v>
@@ -1952,134 +1958,130 @@
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="F34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G34" s="6" t="s">
-        <v>93</v>
+      <c r="G34" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="D35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="F36" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="5" t="s">
-        <v>123</v>
-      </c>
+      <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G38" s="5" t="s">
-        <v>98</v>
+      <c r="G38" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G39" s="6" t="s">
-        <v>102</v>
+      <c r="G39" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>52</v>
@@ -2091,70 +2093,72 @@
         <v>33</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="E41" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>110</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G42" s="5"/>
+      <c r="G42" s="6" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>25</v>
@@ -2163,49 +2167,51 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="B45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F44" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G44" s="5" t="s">
+      <c r="F45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="5" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>52</v>
@@ -2219,94 +2225,94 @@
         <v>25</v>
       </c>
       <c r="G46" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="8" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
       <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="E50" s="5" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>52</v>
@@ -2320,12 +2326,12 @@
         <v>25</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>52</v>
@@ -2333,35 +2339,37 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G52" s="5" t="s">
+      <c r="F53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>147</v>
-      </c>
-      <c r="B53" t="s">
-        <v>52</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
@@ -2373,12 +2381,12 @@
         <v>25</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s">
         <v>52</v>
@@ -2390,12 +2398,12 @@
         <v>25</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B56" t="s">
         <v>52</v>
@@ -2407,12 +2415,12 @@
         <v>25</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s">
         <v>52</v>
@@ -2424,12 +2432,12 @@
         <v>25</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B58" t="s">
         <v>52</v>
@@ -2441,12 +2449,12 @@
         <v>25</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B59" t="s">
         <v>52</v>
@@ -2458,12 +2466,12 @@
         <v>25</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" t="s">
         <v>52</v>
@@ -2475,12 +2483,12 @@
         <v>25</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
@@ -2492,12 +2500,12 @@
         <v>25</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B62" t="s">
         <v>52</v>
@@ -2509,12 +2517,12 @@
         <v>25</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B63" t="s">
         <v>52</v>
@@ -2526,12 +2534,12 @@
         <v>25</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B64" t="s">
         <v>52</v>
@@ -2543,12 +2551,12 @@
         <v>25</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B65" t="s">
         <v>52</v>
@@ -2560,12 +2568,12 @@
         <v>25</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B66" t="s">
         <v>52</v>
@@ -2577,12 +2585,12 @@
         <v>25</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
@@ -2594,12 +2602,12 @@
         <v>25</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B68" t="s">
         <v>52</v>
@@ -2611,12 +2619,12 @@
         <v>25</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B69" t="s">
         <v>52</v>
@@ -2628,12 +2636,12 @@
         <v>25</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B70" t="s">
         <v>52</v>
@@ -2645,12 +2653,12 @@
         <v>25</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B71" t="s">
         <v>52</v>
@@ -2662,12 +2670,12 @@
         <v>25</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B72" t="s">
         <v>52</v>
@@ -2679,12 +2687,12 @@
         <v>25</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
@@ -2696,12 +2704,12 @@
         <v>25</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B74" t="s">
         <v>52</v>
@@ -2713,12 +2721,12 @@
         <v>25</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B75" t="s">
         <v>52</v>
@@ -2730,12 +2738,12 @@
         <v>25</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B76" t="s">
         <v>52</v>
@@ -2747,12 +2755,12 @@
         <v>25</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B77" t="s">
         <v>52</v>
@@ -2764,12 +2772,12 @@
         <v>25</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B78" t="s">
         <v>52</v>
@@ -2781,12 +2789,12 @@
         <v>25</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B79" t="s">
         <v>52</v>
@@ -2798,46 +2806,46 @@
         <v>25</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>173</v>
+      </c>
+      <c r="B80" t="s">
+        <v>52</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>174</v>
       </c>
-      <c r="B80" t="s">
-        <v>52</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G80" s="10" t="s">
+      <c r="B81" t="s">
+        <v>52</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" s="10" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B81" t="s">
-        <v>52</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G81" s="10" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B82" t="s">
         <v>52</v>
@@ -2849,12 +2857,12 @@
         <v>25</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B83" t="s">
         <v>52</v>
@@ -2866,12 +2874,12 @@
         <v>25</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B84" t="s">
         <v>52</v>
@@ -2883,12 +2891,12 @@
         <v>25</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B85" t="s">
         <v>52</v>
@@ -2900,12 +2908,12 @@
         <v>25</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B86" t="s">
         <v>52</v>
@@ -2917,12 +2925,12 @@
         <v>25</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B87" t="s">
         <v>52</v>
@@ -2934,12 +2942,12 @@
         <v>25</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B88" t="s">
         <v>52</v>
@@ -2951,12 +2959,12 @@
         <v>25</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B89" t="s">
         <v>52</v>
@@ -2968,12 +2976,12 @@
         <v>25</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B90" t="s">
         <v>52</v>
@@ -2985,12 +2993,12 @@
         <v>25</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B91" t="s">
         <v>52</v>
@@ -3002,12 +3010,12 @@
         <v>25</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B92" t="s">
         <v>52</v>
@@ -3019,12 +3027,12 @@
         <v>25</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B93" t="s">
         <v>52</v>
@@ -3036,12 +3044,12 @@
         <v>25</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B94" t="s">
         <v>52</v>
@@ -3053,12 +3061,12 @@
         <v>25</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B95" t="s">
         <v>52</v>
@@ -3070,12 +3078,12 @@
         <v>25</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B96" t="s">
         <v>52</v>
@@ -3087,12 +3095,12 @@
         <v>25</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B97" t="s">
         <v>52</v>
@@ -3104,12 +3112,12 @@
         <v>25</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B98" t="s">
         <v>52</v>
@@ -3121,12 +3129,12 @@
         <v>25</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B99" t="s">
         <v>52</v>
@@ -3138,12 +3146,12 @@
         <v>25</v>
       </c>
       <c r="G99" s="10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B100" t="s">
         <v>52</v>
@@ -3155,12 +3163,12 @@
         <v>25</v>
       </c>
       <c r="G100" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B101" t="s">
         <v>52</v>
@@ -3172,12 +3180,12 @@
         <v>25</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B102" t="s">
         <v>52</v>
@@ -3189,12 +3197,12 @@
         <v>25</v>
       </c>
       <c r="G102" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B103" t="s">
         <v>52</v>
@@ -3206,12 +3214,12 @@
         <v>25</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B104" t="s">
         <v>52</v>
@@ -3223,12 +3231,12 @@
         <v>25</v>
       </c>
       <c r="G104" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B105" t="s">
         <v>52</v>
@@ -3240,12 +3248,12 @@
         <v>25</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B106" t="s">
         <v>52</v>
@@ -3257,12 +3265,12 @@
         <v>25</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B107" t="s">
         <v>52</v>
@@ -3274,12 +3282,12 @@
         <v>25</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B108" t="s">
         <v>52</v>
@@ -3291,12 +3299,12 @@
         <v>25</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B109" t="s">
         <v>52</v>
@@ -3308,12 +3316,12 @@
         <v>25</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B110" t="s">
         <v>52</v>
@@ -3325,12 +3333,12 @@
         <v>25</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B111" t="s">
         <v>52</v>
@@ -3342,12 +3350,12 @@
         <v>25</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B112" t="s">
         <v>52</v>
@@ -3359,46 +3367,46 @@
         <v>25</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B113" t="s">
+        <v>52</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G113" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="B113" t="s">
-        <v>52</v>
-      </c>
-      <c r="E113" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F113" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G113" s="10" t="s">
+      <c r="B114" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G114" s="10" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>274</v>
-      </c>
-      <c r="B114" t="s">
-        <v>52</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F114" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G114" s="10" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B115" t="s">
         <v>52</v>
@@ -3410,12 +3418,12 @@
         <v>25</v>
       </c>
       <c r="G115" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B116" t="s">
         <v>52</v>
@@ -3427,12 +3435,12 @@
         <v>25</v>
       </c>
       <c r="G116" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B117" t="s">
         <v>52</v>
@@ -3444,12 +3452,12 @@
         <v>25</v>
       </c>
       <c r="G117" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B118" t="s">
         <v>52</v>
@@ -3461,23 +3469,40 @@
         <v>25</v>
       </c>
       <c r="G118" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>278</v>
+      </c>
+      <c r="B119" t="s">
+        <v>52</v>
+      </c>
+      <c r="E119" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F119" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G119" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>279</v>
       </c>
-      <c r="B119" t="s">
-        <v>52</v>
-      </c>
-      <c r="E119" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F119" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G119" s="10" t="s">
+      <c r="B120" t="s">
+        <v>52</v>
+      </c>
+      <c r="E120" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F120" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G120" s="10" t="s">
         <v>285</v>
       </c>
     </row>
@@ -3487,84 +3512,84 @@
     <hyperlink ref="G14" r:id="rId2"/>
     <hyperlink ref="G13" r:id="rId3"/>
     <hyperlink ref="G12" r:id="rId4"/>
-    <hyperlink ref="G34" r:id="rId5"/>
-    <hyperlink ref="G35" r:id="rId6"/>
-    <hyperlink ref="G36" r:id="rId7"/>
-    <hyperlink ref="G37" r:id="rId8"/>
-    <hyperlink ref="G39" r:id="rId9"/>
-    <hyperlink ref="G40" r:id="rId10"/>
-    <hyperlink ref="G41" r:id="rId11"/>
-    <hyperlink ref="G45" r:id="rId12"/>
-    <hyperlink ref="G46" r:id="rId13"/>
-    <hyperlink ref="G47" r:id="rId14"/>
-    <hyperlink ref="G48" r:id="rId15"/>
-    <hyperlink ref="G49" r:id="rId16"/>
-    <hyperlink ref="G51" r:id="rId17"/>
-    <hyperlink ref="G55" r:id="rId18"/>
-    <hyperlink ref="G54" r:id="rId19"/>
-    <hyperlink ref="G56" r:id="rId20"/>
-    <hyperlink ref="G57" r:id="rId21"/>
-    <hyperlink ref="G58" r:id="rId22"/>
-    <hyperlink ref="G59" r:id="rId23"/>
-    <hyperlink ref="G60" r:id="rId24"/>
-    <hyperlink ref="G61" r:id="rId25"/>
-    <hyperlink ref="G62" r:id="rId26"/>
-    <hyperlink ref="G63" r:id="rId27"/>
-    <hyperlink ref="G64" r:id="rId28"/>
-    <hyperlink ref="G65" r:id="rId29"/>
-    <hyperlink ref="G66" r:id="rId30"/>
-    <hyperlink ref="G67" r:id="rId31"/>
-    <hyperlink ref="G68" r:id="rId32"/>
-    <hyperlink ref="G69" r:id="rId33"/>
-    <hyperlink ref="G53" r:id="rId34"/>
-    <hyperlink ref="G70" r:id="rId35"/>
-    <hyperlink ref="G71" r:id="rId36"/>
-    <hyperlink ref="G72" r:id="rId37"/>
-    <hyperlink ref="G73" r:id="rId38"/>
-    <hyperlink ref="G74" r:id="rId39"/>
-    <hyperlink ref="G75" r:id="rId40"/>
-    <hyperlink ref="G76" r:id="rId41"/>
-    <hyperlink ref="G77" r:id="rId42"/>
-    <hyperlink ref="G78" r:id="rId43"/>
-    <hyperlink ref="G79" r:id="rId44"/>
-    <hyperlink ref="G80" r:id="rId45"/>
-    <hyperlink ref="G82" r:id="rId46"/>
-    <hyperlink ref="G83" r:id="rId47"/>
-    <hyperlink ref="G84" r:id="rId48"/>
-    <hyperlink ref="G85" r:id="rId49"/>
-    <hyperlink ref="G86" r:id="rId50"/>
-    <hyperlink ref="G87" r:id="rId51"/>
-    <hyperlink ref="G88" r:id="rId52"/>
-    <hyperlink ref="G89" r:id="rId53"/>
-    <hyperlink ref="G90" r:id="rId54"/>
-    <hyperlink ref="G91" r:id="rId55"/>
-    <hyperlink ref="G92" r:id="rId56"/>
-    <hyperlink ref="G93" r:id="rId57"/>
-    <hyperlink ref="G94" r:id="rId58"/>
-    <hyperlink ref="G95" r:id="rId59"/>
-    <hyperlink ref="G96" r:id="rId60"/>
-    <hyperlink ref="G97" r:id="rId61"/>
-    <hyperlink ref="G98" r:id="rId62"/>
-    <hyperlink ref="G99" r:id="rId63"/>
-    <hyperlink ref="G100" r:id="rId64"/>
-    <hyperlink ref="G101" r:id="rId65"/>
-    <hyperlink ref="G102" r:id="rId66"/>
-    <hyperlink ref="G103" r:id="rId67"/>
-    <hyperlink ref="G104" r:id="rId68"/>
-    <hyperlink ref="G105" r:id="rId69"/>
-    <hyperlink ref="G106" r:id="rId70"/>
-    <hyperlink ref="G107" r:id="rId71"/>
-    <hyperlink ref="G108" r:id="rId72"/>
-    <hyperlink ref="G109" r:id="rId73"/>
-    <hyperlink ref="G110" r:id="rId74"/>
-    <hyperlink ref="G113" r:id="rId75"/>
-    <hyperlink ref="G111" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
-    <hyperlink ref="G114" r:id="rId77"/>
-    <hyperlink ref="G115" r:id="rId78"/>
-    <hyperlink ref="G116" r:id="rId79"/>
-    <hyperlink ref="G117" r:id="rId80"/>
-    <hyperlink ref="G118" r:id="rId81"/>
-    <hyperlink ref="G119" r:id="rId82"/>
+    <hyperlink ref="G35" r:id="rId5"/>
+    <hyperlink ref="G36" r:id="rId6"/>
+    <hyperlink ref="G37" r:id="rId7"/>
+    <hyperlink ref="G38" r:id="rId8"/>
+    <hyperlink ref="G40" r:id="rId9"/>
+    <hyperlink ref="G41" r:id="rId10"/>
+    <hyperlink ref="G42" r:id="rId11"/>
+    <hyperlink ref="G46" r:id="rId12"/>
+    <hyperlink ref="G47" r:id="rId13"/>
+    <hyperlink ref="G48" r:id="rId14"/>
+    <hyperlink ref="G49" r:id="rId15"/>
+    <hyperlink ref="G50" r:id="rId16"/>
+    <hyperlink ref="G52" r:id="rId17"/>
+    <hyperlink ref="G56" r:id="rId18"/>
+    <hyperlink ref="G55" r:id="rId19"/>
+    <hyperlink ref="G57" r:id="rId20"/>
+    <hyperlink ref="G58" r:id="rId21"/>
+    <hyperlink ref="G59" r:id="rId22"/>
+    <hyperlink ref="G60" r:id="rId23"/>
+    <hyperlink ref="G61" r:id="rId24"/>
+    <hyperlink ref="G62" r:id="rId25"/>
+    <hyperlink ref="G63" r:id="rId26"/>
+    <hyperlink ref="G64" r:id="rId27"/>
+    <hyperlink ref="G65" r:id="rId28"/>
+    <hyperlink ref="G66" r:id="rId29"/>
+    <hyperlink ref="G67" r:id="rId30"/>
+    <hyperlink ref="G68" r:id="rId31"/>
+    <hyperlink ref="G69" r:id="rId32"/>
+    <hyperlink ref="G70" r:id="rId33"/>
+    <hyperlink ref="G54" r:id="rId34"/>
+    <hyperlink ref="G71" r:id="rId35"/>
+    <hyperlink ref="G72" r:id="rId36"/>
+    <hyperlink ref="G73" r:id="rId37"/>
+    <hyperlink ref="G74" r:id="rId38"/>
+    <hyperlink ref="G75" r:id="rId39"/>
+    <hyperlink ref="G76" r:id="rId40"/>
+    <hyperlink ref="G77" r:id="rId41"/>
+    <hyperlink ref="G78" r:id="rId42"/>
+    <hyperlink ref="G79" r:id="rId43"/>
+    <hyperlink ref="G80" r:id="rId44"/>
+    <hyperlink ref="G81" r:id="rId45"/>
+    <hyperlink ref="G83" r:id="rId46"/>
+    <hyperlink ref="G84" r:id="rId47"/>
+    <hyperlink ref="G85" r:id="rId48"/>
+    <hyperlink ref="G86" r:id="rId49"/>
+    <hyperlink ref="G87" r:id="rId50"/>
+    <hyperlink ref="G88" r:id="rId51"/>
+    <hyperlink ref="G89" r:id="rId52"/>
+    <hyperlink ref="G90" r:id="rId53"/>
+    <hyperlink ref="G91" r:id="rId54"/>
+    <hyperlink ref="G92" r:id="rId55"/>
+    <hyperlink ref="G93" r:id="rId56"/>
+    <hyperlink ref="G94" r:id="rId57"/>
+    <hyperlink ref="G95" r:id="rId58"/>
+    <hyperlink ref="G96" r:id="rId59"/>
+    <hyperlink ref="G97" r:id="rId60"/>
+    <hyperlink ref="G98" r:id="rId61"/>
+    <hyperlink ref="G99" r:id="rId62"/>
+    <hyperlink ref="G100" r:id="rId63"/>
+    <hyperlink ref="G101" r:id="rId64"/>
+    <hyperlink ref="G102" r:id="rId65"/>
+    <hyperlink ref="G103" r:id="rId66"/>
+    <hyperlink ref="G104" r:id="rId67"/>
+    <hyperlink ref="G105" r:id="rId68"/>
+    <hyperlink ref="G106" r:id="rId69"/>
+    <hyperlink ref="G107" r:id="rId70"/>
+    <hyperlink ref="G108" r:id="rId71"/>
+    <hyperlink ref="G109" r:id="rId72"/>
+    <hyperlink ref="G110" r:id="rId73"/>
+    <hyperlink ref="G111" r:id="rId74"/>
+    <hyperlink ref="G114" r:id="rId75"/>
+    <hyperlink ref="G112" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
+    <hyperlink ref="G115" r:id="rId77"/>
+    <hyperlink ref="G116" r:id="rId78"/>
+    <hyperlink ref="G117" r:id="rId79"/>
+    <hyperlink ref="G118" r:id="rId80"/>
+    <hyperlink ref="G119" r:id="rId81"/>
+    <hyperlink ref="G120" r:id="rId82"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId83"/>
@@ -3581,8 +3606,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Oleg Babak - fix for user for Firm Style Smoke test
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C793437
</commit_message>
<xml_diff>
--- a/PPIUK-SmokeTest/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-SmokeTest/src/test/resources/CobaltUsers.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Emails" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="294">
   <si>
     <t>UserName</t>
   </si>
@@ -889,13 +889,23 @@
   </si>
   <si>
     <t>firmstyle@mailinator.com</t>
+  </si>
+  <si>
+    <t>Password1234!</t>
+  </si>
+  <si>
+    <t>Firm Style user</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1309,20 +1319,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1944,17 +1954,15 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
-        <v>75</v>
+        <v>292</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>25</v>
@@ -1963,10 +1971,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>74</v>
+        <v>284</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>52</v>
+        <v>285</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5" t="s">
@@ -1982,26 +1990,26 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="E34" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>83</v>
-      </c>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>81</v>
@@ -2009,134 +2017,130 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="F36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="6" t="s">
-        <v>92</v>
+      <c r="G36" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5" t="s">
-        <v>91</v>
-      </c>
+      <c r="D37" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="F38" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="5" t="s">
-        <v>122</v>
-      </c>
+      <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G40" s="5" t="s">
-        <v>97</v>
+      <c r="G40" s="6" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>101</v>
+      <c r="G41" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>52</v>
@@ -2148,70 +2152,72 @@
         <v>33</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="E43" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>109</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G44" s="5"/>
+      <c r="G44" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>25</v>
@@ -2220,49 +2226,51 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="5" t="s">
+      <c r="B47" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D47" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F46" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G46" s="5" t="s">
+      <c r="F47" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>52</v>
@@ -2276,94 +2284,94 @@
         <v>25</v>
       </c>
       <c r="G48" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="8" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
       <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="E52" s="5" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>52</v>
@@ -2377,12 +2385,12 @@
         <v>25</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>52</v>
@@ -2390,35 +2398,37 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F54" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G54" s="5" t="s">
+      <c r="F55" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>145</v>
-      </c>
-      <c r="B55" t="s">
-        <v>52</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s">
         <v>52</v>
@@ -2430,12 +2440,12 @@
         <v>25</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
         <v>52</v>
@@ -2447,12 +2457,12 @@
         <v>25</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B58" t="s">
         <v>52</v>
@@ -2464,12 +2474,12 @@
         <v>25</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B59" t="s">
         <v>52</v>
@@ -2481,12 +2491,12 @@
         <v>25</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B60" t="s">
         <v>52</v>
@@ -2498,12 +2508,12 @@
         <v>25</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
@@ -2515,12 +2525,12 @@
         <v>25</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B62" t="s">
         <v>52</v>
@@ -2532,12 +2542,12 @@
         <v>25</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
         <v>52</v>
@@ -2549,12 +2559,12 @@
         <v>25</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B64" t="s">
         <v>52</v>
@@ -2566,12 +2576,12 @@
         <v>25</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B65" t="s">
         <v>52</v>
@@ -2583,12 +2593,12 @@
         <v>25</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B66" t="s">
         <v>52</v>
@@ -2600,12 +2610,12 @@
         <v>25</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
@@ -2617,12 +2627,12 @@
         <v>25</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B68" t="s">
         <v>52</v>
@@ -2634,12 +2644,12 @@
         <v>25</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B69" t="s">
         <v>52</v>
@@ -2651,12 +2661,12 @@
         <v>25</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B70" t="s">
         <v>52</v>
@@ -2668,12 +2678,12 @@
         <v>25</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B71" t="s">
         <v>52</v>
@@ -2685,12 +2695,12 @@
         <v>25</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B72" t="s">
         <v>52</v>
@@ -2702,12 +2712,12 @@
         <v>25</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
@@ -2719,12 +2729,12 @@
         <v>25</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B74" t="s">
         <v>52</v>
@@ -2736,12 +2746,12 @@
         <v>25</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B75" t="s">
         <v>52</v>
@@ -2753,12 +2763,12 @@
         <v>25</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B76" t="s">
         <v>52</v>
@@ -2770,12 +2780,12 @@
         <v>25</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B77" t="s">
         <v>52</v>
@@ -2787,12 +2797,12 @@
         <v>25</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B78" t="s">
         <v>52</v>
@@ -2804,12 +2814,12 @@
         <v>25</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B79" t="s">
         <v>52</v>
@@ -2821,12 +2831,12 @@
         <v>25</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B80" t="s">
         <v>52</v>
@@ -2838,12 +2848,12 @@
         <v>25</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B81" t="s">
         <v>52</v>
@@ -2855,46 +2865,46 @@
         <v>25</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>171</v>
+      </c>
+      <c r="B82" t="s">
+        <v>52</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>172</v>
       </c>
-      <c r="B82" t="s">
-        <v>52</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G82" s="10" t="s">
+      <c r="B83" t="s">
+        <v>52</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G83" s="10" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="B83" t="s">
-        <v>52</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G83" s="10" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B84" t="s">
         <v>52</v>
@@ -2906,12 +2916,12 @@
         <v>25</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B85" t="s">
         <v>52</v>
@@ -2923,12 +2933,12 @@
         <v>25</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B86" t="s">
         <v>52</v>
@@ -2940,12 +2950,12 @@
         <v>25</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B87" t="s">
         <v>52</v>
@@ -2957,12 +2967,12 @@
         <v>25</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B88" t="s">
         <v>52</v>
@@ -2974,12 +2984,12 @@
         <v>25</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B89" t="s">
         <v>52</v>
@@ -2991,12 +3001,12 @@
         <v>25</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B90" t="s">
         <v>52</v>
@@ -3008,12 +3018,12 @@
         <v>25</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B91" t="s">
         <v>52</v>
@@ -3025,12 +3035,12 @@
         <v>25</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B92" t="s">
         <v>52</v>
@@ -3042,12 +3052,12 @@
         <v>25</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B93" t="s">
         <v>52</v>
@@ -3059,12 +3069,12 @@
         <v>25</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B94" t="s">
         <v>52</v>
@@ -3076,12 +3086,12 @@
         <v>25</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B95" t="s">
         <v>52</v>
@@ -3093,12 +3103,12 @@
         <v>25</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B96" t="s">
         <v>52</v>
@@ -3110,12 +3120,12 @@
         <v>25</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B97" t="s">
         <v>52</v>
@@ -3127,12 +3137,12 @@
         <v>25</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B98" t="s">
         <v>52</v>
@@ -3144,12 +3154,12 @@
         <v>25</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B99" t="s">
         <v>52</v>
@@ -3161,12 +3171,12 @@
         <v>25</v>
       </c>
       <c r="G99" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B100" t="s">
         <v>52</v>
@@ -3178,12 +3188,12 @@
         <v>25</v>
       </c>
       <c r="G100" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B101" t="s">
         <v>52</v>
@@ -3195,12 +3205,12 @@
         <v>25</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B102" t="s">
         <v>52</v>
@@ -3212,12 +3222,12 @@
         <v>25</v>
       </c>
       <c r="G102" s="10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B103" t="s">
         <v>52</v>
@@ -3229,12 +3239,12 @@
         <v>25</v>
       </c>
       <c r="G103" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B104" t="s">
         <v>52</v>
@@ -3246,12 +3256,12 @@
         <v>25</v>
       </c>
       <c r="G104" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B105" t="s">
         <v>52</v>
@@ -3263,12 +3273,12 @@
         <v>25</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B106" t="s">
         <v>52</v>
@@ -3280,12 +3290,12 @@
         <v>25</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B107" t="s">
         <v>52</v>
@@ -3297,12 +3307,12 @@
         <v>25</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B108" t="s">
         <v>52</v>
@@ -3314,12 +3324,12 @@
         <v>25</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B109" t="s">
         <v>52</v>
@@ -3331,12 +3341,12 @@
         <v>25</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B110" t="s">
         <v>52</v>
@@ -3348,12 +3358,12 @@
         <v>25</v>
       </c>
       <c r="G110" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B111" t="s">
         <v>52</v>
@@ -3365,12 +3375,12 @@
         <v>25</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B112" t="s">
         <v>52</v>
@@ -3382,12 +3392,12 @@
         <v>25</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B113" t="s">
         <v>52</v>
@@ -3399,12 +3409,12 @@
         <v>25</v>
       </c>
       <c r="G113" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B114" t="s">
         <v>52</v>
@@ -3416,46 +3426,46 @@
         <v>25</v>
       </c>
       <c r="G114" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="B115" t="s">
+        <v>52</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G115" s="10" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="B115" t="s">
-        <v>52</v>
-      </c>
-      <c r="E115" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F115" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G115" s="10" t="s">
+      <c r="B116" t="s">
+        <v>52</v>
+      </c>
+      <c r="E116" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G116" s="10" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>272</v>
-      </c>
-      <c r="B116" t="s">
-        <v>52</v>
-      </c>
-      <c r="E116" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F116" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G116" s="10" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B117" t="s">
         <v>52</v>
@@ -3467,12 +3477,12 @@
         <v>25</v>
       </c>
       <c r="G117" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B118" t="s">
         <v>52</v>
@@ -3484,12 +3494,12 @@
         <v>25</v>
       </c>
       <c r="G118" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B119" t="s">
         <v>52</v>
@@ -3501,12 +3511,12 @@
         <v>25</v>
       </c>
       <c r="G119" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B120" t="s">
         <v>52</v>
@@ -3518,23 +3528,40 @@
         <v>25</v>
       </c>
       <c r="G120" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>276</v>
+      </c>
+      <c r="B121" t="s">
+        <v>52</v>
+      </c>
+      <c r="E121" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F121" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G121" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>277</v>
       </c>
-      <c r="B121" t="s">
-        <v>52</v>
-      </c>
-      <c r="E121" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F121" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G121" s="10" t="s">
+      <c r="B122" t="s">
+        <v>52</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F122" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G122" s="10" t="s">
         <v>283</v>
       </c>
     </row>
@@ -3544,84 +3571,84 @@
     <hyperlink ref="G15" r:id="rId2"/>
     <hyperlink ref="G14" r:id="rId3"/>
     <hyperlink ref="G13" r:id="rId4"/>
-    <hyperlink ref="G36" r:id="rId5"/>
-    <hyperlink ref="G37" r:id="rId6"/>
-    <hyperlink ref="G38" r:id="rId7"/>
-    <hyperlink ref="G39" r:id="rId8"/>
-    <hyperlink ref="G41" r:id="rId9"/>
-    <hyperlink ref="G42" r:id="rId10"/>
-    <hyperlink ref="G43" r:id="rId11"/>
-    <hyperlink ref="G47" r:id="rId12"/>
-    <hyperlink ref="G48" r:id="rId13"/>
-    <hyperlink ref="G49" r:id="rId14"/>
-    <hyperlink ref="G50" r:id="rId15"/>
-    <hyperlink ref="G51" r:id="rId16"/>
-    <hyperlink ref="G53" r:id="rId17"/>
-    <hyperlink ref="G57" r:id="rId18"/>
-    <hyperlink ref="G56" r:id="rId19"/>
-    <hyperlink ref="G58" r:id="rId20"/>
-    <hyperlink ref="G59" r:id="rId21"/>
-    <hyperlink ref="G60" r:id="rId22"/>
-    <hyperlink ref="G61" r:id="rId23"/>
-    <hyperlink ref="G62" r:id="rId24"/>
-    <hyperlink ref="G63" r:id="rId25"/>
-    <hyperlink ref="G64" r:id="rId26"/>
-    <hyperlink ref="G65" r:id="rId27"/>
-    <hyperlink ref="G66" r:id="rId28"/>
-    <hyperlink ref="G67" r:id="rId29"/>
-    <hyperlink ref="G68" r:id="rId30"/>
-    <hyperlink ref="G69" r:id="rId31"/>
-    <hyperlink ref="G70" r:id="rId32"/>
-    <hyperlink ref="G71" r:id="rId33"/>
-    <hyperlink ref="G55" r:id="rId34"/>
-    <hyperlink ref="G72" r:id="rId35"/>
-    <hyperlink ref="G73" r:id="rId36"/>
-    <hyperlink ref="G74" r:id="rId37"/>
-    <hyperlink ref="G75" r:id="rId38"/>
-    <hyperlink ref="G76" r:id="rId39"/>
-    <hyperlink ref="G77" r:id="rId40"/>
-    <hyperlink ref="G78" r:id="rId41"/>
-    <hyperlink ref="G79" r:id="rId42"/>
-    <hyperlink ref="G80" r:id="rId43"/>
-    <hyperlink ref="G81" r:id="rId44"/>
-    <hyperlink ref="G82" r:id="rId45"/>
-    <hyperlink ref="G84" r:id="rId46"/>
-    <hyperlink ref="G85" r:id="rId47"/>
-    <hyperlink ref="G86" r:id="rId48"/>
-    <hyperlink ref="G87" r:id="rId49"/>
-    <hyperlink ref="G88" r:id="rId50"/>
-    <hyperlink ref="G89" r:id="rId51"/>
-    <hyperlink ref="G90" r:id="rId52"/>
-    <hyperlink ref="G91" r:id="rId53"/>
-    <hyperlink ref="G92" r:id="rId54"/>
-    <hyperlink ref="G93" r:id="rId55"/>
-    <hyperlink ref="G94" r:id="rId56"/>
-    <hyperlink ref="G95" r:id="rId57"/>
-    <hyperlink ref="G96" r:id="rId58"/>
-    <hyperlink ref="G97" r:id="rId59"/>
-    <hyperlink ref="G98" r:id="rId60"/>
-    <hyperlink ref="G99" r:id="rId61"/>
-    <hyperlink ref="G100" r:id="rId62"/>
-    <hyperlink ref="G101" r:id="rId63"/>
-    <hyperlink ref="G102" r:id="rId64"/>
-    <hyperlink ref="G103" r:id="rId65"/>
-    <hyperlink ref="G104" r:id="rId66"/>
-    <hyperlink ref="G105" r:id="rId67"/>
-    <hyperlink ref="G106" r:id="rId68"/>
-    <hyperlink ref="G107" r:id="rId69"/>
-    <hyperlink ref="G108" r:id="rId70"/>
-    <hyperlink ref="G109" r:id="rId71"/>
-    <hyperlink ref="G110" r:id="rId72"/>
-    <hyperlink ref="G111" r:id="rId73"/>
-    <hyperlink ref="G112" r:id="rId74"/>
-    <hyperlink ref="G115" r:id="rId75"/>
-    <hyperlink ref="G113" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
-    <hyperlink ref="G116" r:id="rId77"/>
-    <hyperlink ref="G117" r:id="rId78"/>
-    <hyperlink ref="G118" r:id="rId79"/>
-    <hyperlink ref="G119" r:id="rId80"/>
-    <hyperlink ref="G120" r:id="rId81"/>
-    <hyperlink ref="G121" r:id="rId82"/>
+    <hyperlink ref="G37" r:id="rId5"/>
+    <hyperlink ref="G38" r:id="rId6"/>
+    <hyperlink ref="G39" r:id="rId7"/>
+    <hyperlink ref="G40" r:id="rId8"/>
+    <hyperlink ref="G42" r:id="rId9"/>
+    <hyperlink ref="G43" r:id="rId10"/>
+    <hyperlink ref="G44" r:id="rId11"/>
+    <hyperlink ref="G48" r:id="rId12"/>
+    <hyperlink ref="G49" r:id="rId13"/>
+    <hyperlink ref="G50" r:id="rId14"/>
+    <hyperlink ref="G51" r:id="rId15"/>
+    <hyperlink ref="G52" r:id="rId16"/>
+    <hyperlink ref="G54" r:id="rId17"/>
+    <hyperlink ref="G58" r:id="rId18"/>
+    <hyperlink ref="G57" r:id="rId19"/>
+    <hyperlink ref="G59" r:id="rId20"/>
+    <hyperlink ref="G60" r:id="rId21"/>
+    <hyperlink ref="G61" r:id="rId22"/>
+    <hyperlink ref="G62" r:id="rId23"/>
+    <hyperlink ref="G63" r:id="rId24"/>
+    <hyperlink ref="G64" r:id="rId25"/>
+    <hyperlink ref="G65" r:id="rId26"/>
+    <hyperlink ref="G66" r:id="rId27"/>
+    <hyperlink ref="G67" r:id="rId28"/>
+    <hyperlink ref="G68" r:id="rId29"/>
+    <hyperlink ref="G69" r:id="rId30"/>
+    <hyperlink ref="G70" r:id="rId31"/>
+    <hyperlink ref="G71" r:id="rId32"/>
+    <hyperlink ref="G72" r:id="rId33"/>
+    <hyperlink ref="G56" r:id="rId34"/>
+    <hyperlink ref="G73" r:id="rId35"/>
+    <hyperlink ref="G74" r:id="rId36"/>
+    <hyperlink ref="G75" r:id="rId37"/>
+    <hyperlink ref="G76" r:id="rId38"/>
+    <hyperlink ref="G77" r:id="rId39"/>
+    <hyperlink ref="G78" r:id="rId40"/>
+    <hyperlink ref="G79" r:id="rId41"/>
+    <hyperlink ref="G80" r:id="rId42"/>
+    <hyperlink ref="G81" r:id="rId43"/>
+    <hyperlink ref="G82" r:id="rId44"/>
+    <hyperlink ref="G83" r:id="rId45"/>
+    <hyperlink ref="G85" r:id="rId46"/>
+    <hyperlink ref="G86" r:id="rId47"/>
+    <hyperlink ref="G87" r:id="rId48"/>
+    <hyperlink ref="G88" r:id="rId49"/>
+    <hyperlink ref="G89" r:id="rId50"/>
+    <hyperlink ref="G90" r:id="rId51"/>
+    <hyperlink ref="G91" r:id="rId52"/>
+    <hyperlink ref="G92" r:id="rId53"/>
+    <hyperlink ref="G93" r:id="rId54"/>
+    <hyperlink ref="G94" r:id="rId55"/>
+    <hyperlink ref="G95" r:id="rId56"/>
+    <hyperlink ref="G96" r:id="rId57"/>
+    <hyperlink ref="G97" r:id="rId58"/>
+    <hyperlink ref="G98" r:id="rId59"/>
+    <hyperlink ref="G99" r:id="rId60"/>
+    <hyperlink ref="G100" r:id="rId61"/>
+    <hyperlink ref="G101" r:id="rId62"/>
+    <hyperlink ref="G102" r:id="rId63"/>
+    <hyperlink ref="G103" r:id="rId64"/>
+    <hyperlink ref="G104" r:id="rId65"/>
+    <hyperlink ref="G105" r:id="rId66"/>
+    <hyperlink ref="G106" r:id="rId67"/>
+    <hyperlink ref="G107" r:id="rId68"/>
+    <hyperlink ref="G108" r:id="rId69"/>
+    <hyperlink ref="G109" r:id="rId70"/>
+    <hyperlink ref="G110" r:id="rId71"/>
+    <hyperlink ref="G111" r:id="rId72"/>
+    <hyperlink ref="G112" r:id="rId73"/>
+    <hyperlink ref="G113" r:id="rId74"/>
+    <hyperlink ref="G116" r:id="rId75"/>
+    <hyperlink ref="G114" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
+    <hyperlink ref="G117" r:id="rId77"/>
+    <hyperlink ref="G118" r:id="rId78"/>
+    <hyperlink ref="G119" r:id="rId79"/>
+    <hyperlink ref="G120" r:id="rId80"/>
+    <hyperlink ref="G121" r:id="rId81"/>
+    <hyperlink ref="G122" r:id="rId82"/>
     <hyperlink ref="G10" r:id="rId83"/>
     <hyperlink ref="G9" r:id="rId84"/>
   </hyperlinks>
@@ -3640,8 +3667,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Oleg Babak - update Oleg_Babak user in CobaltUsers.xlsx for PPIUK-SmokeTest
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C794261
</commit_message>
<xml_diff>
--- a/PPIUK-SmokeTest/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-SmokeTest/src/test/resources/CobaltUsers.xlsx
@@ -873,9 +873,6 @@
     <t>Oleg_Babak</t>
   </si>
   <si>
-    <t>Password1!</t>
-  </si>
-  <si>
     <t>FSTestUser2</t>
   </si>
   <si>
@@ -892,6 +889,9 @@
   </si>
   <si>
     <t>Password12345</t>
+  </si>
+  <si>
+    <t>Password10!</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1315,7 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,10 +1496,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1512,15 +1512,15 @@
         <v>25</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1533,7 +1533,7 @@
         <v>25</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1950,7 +1950,7 @@
         <v>284</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">

</xml_diff>

<commit_message>
Oleg Babak - password updated for Smoke test user
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C794519
</commit_message>
<xml_diff>
--- a/PPIUK-SmokeTest/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-SmokeTest/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="293">
   <si>
     <t>UserName</t>
   </si>
@@ -891,7 +891,10 @@
     <t>Password12345</t>
   </si>
   <si>
-    <t>Password11!</t>
+    <t>Passw0rd!</t>
+  </si>
+  <si>
+    <t>Smoke Test User (DO NOT USE OR UPDATE)</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1318,7 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,7 +1960,7 @@
         <v>21</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>75</v>
+        <v>292</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Oleg Babak - Update CobaltUsers.xlsx
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C795470
</commit_message>
<xml_diff>
--- a/PPIUK-SmokeTest/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-SmokeTest/src/test/resources/CobaltUsers.xlsx
@@ -891,10 +891,10 @@
     <t>Password12345</t>
   </si>
   <si>
-    <t>Passw0rd!</t>
-  </si>
-  <si>
     <t>Smoke Test User (DO NOT USE OR UPDATE)</t>
+  </si>
+  <si>
+    <t>Passw0rd!!</t>
   </si>
 </sst>
 </file>
@@ -1318,7 +1318,7 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,14 +1953,14 @@
         <v>284</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>25</v>

</xml_diff>